<commit_message>
Combat Extended Guns 업데이트
#1214
</commit_message>
<xml_diff>
--- a/Data/Combat Extended/①_Combat Extended Guns - 1582570547/1582570547.xlsx
+++ b/Data/Combat Extended/①_Combat Extended Guns - 1582570547/1582570547.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.7.11\CE Translation\3079466972\Data\Combat Extended\①_Combat Extended Guns - 1582570547\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Combat Extended\①_Combat Extended Guns - 1582570547\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B451DA66-08E4-4A3D-9E7E-B326F0037D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB2F9A3-878D-4F5A-A7F3-FF40096C7E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="38340" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240415" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240726" sheetId="2" r:id="rId1"/>
+    <sheet name="Old_240415" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="696">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1535,13 +1549,599 @@
   </si>
   <si>
     <t>M134 미니건</t>
+  </si>
+  <si>
+    <t>▲▲▲</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닐라 오버라이드</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>▼▼▼</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glock 18</t>
+  </si>
+  <si>
+    <t>Vanilla Weapons Expanded - Quickdraw</t>
+  </si>
+  <si>
+    <t>VWE_Gun_AutomaticPistol.label</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+VWE_Gun_AutomaticPistol.label</t>
+  </si>
+  <si>
+    <t>Bullpup DMR</t>
+  </si>
+  <si>
+    <t>VWE_Gun_BullpupDMR.label</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+VWE_Gun_BullpupDMR.label</t>
+  </si>
+  <si>
+    <t>FAMAS</t>
+  </si>
+  <si>
+    <t>VWE_Gun_BullpupRifle.label</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+VWE_Gun_BullpupRifle.label</t>
+  </si>
+  <si>
+    <t>P90</t>
+  </si>
+  <si>
+    <t>VWE_Gun_PDW.label</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+VWE_Gun_PDW.label</t>
+  </si>
+  <si>
+    <t>M72 LAW 일회용 로켓 발사기 제작 중</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+MakeDisposableRocketLauncher_x1.jobString</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+MakeDisposableRocketLauncher_x1.description</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+MakeDisposableRocketLauncher.jobString</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+MakeDisposableRocketLauncher.description</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE_Gun_Flamethrower.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_Flamethrower.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_Flamethrower.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_Flamethrower.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeAMR.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeAMR.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeAMR.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeAMR.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeAMR.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeAMR.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeLMG.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeLMG.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeLMG.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeLMG.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeLMG.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeLMG.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeSniperRifle.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeSniperRifle.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeSniperRifle.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeSniperRifle.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeSniperRifle.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeSniperRifle.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeSMG.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeSMG.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeSMG.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeSMG.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeSMG.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeSMG.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeShotgun.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeShotgun.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeShotgun.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeShotgun.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargeShotgun.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargeShotgun.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargePistol.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargePistol.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_ChargePistol.tools.grip.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_ChargePistol.tools.grip.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MilkorMGL.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MilkorMGL.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MilkorMGL.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MilkorMGL.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MilkorMGL.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MilkorMGL.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_RPGSeven.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_RPGSeven.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_PKM.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_PKM.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_PKM.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_PKM.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_PKM.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_PKM.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_RPD.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_RPD.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_RPD.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_RPD.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_RPD.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_RPD.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MSixty.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MSixty.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MSixty.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MSixty.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MSixty.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MSixty.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MTwoFourNine.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MTwoFourNine.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MTwoFourNine.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MTwoFourNine.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_MTwoFourNine.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_MTwoFourNine.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_PTRS.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_PTRS.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_PTRS.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_PTRS.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_PTRS.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_PTRS.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_HecateTwo.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_HecateTwo.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_HecateTwo.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_HecateTwo.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_HecateTwo.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_HecateTwo.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_SVD.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SVD.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_SVD.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SVD.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_SVD.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SVD.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKM.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKM.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKM.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKM.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKM.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKM.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FNFAL.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FNFAL.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FNFAL.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FNFAL.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FNFAL.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FNFAL.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKMSU.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKMSU.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKMSU.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKMSU.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKMSU.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKMSU.tools.stock.label</t>
+  </si>
+  <si>
+    <t>AKMS-U 돌격 소총</t>
+  </si>
+  <si>
+    <t>AKMS-U</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKMSU.verbs.Verb_ShootCE.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKMSU.verbs.Verb_ShootCE.label</t>
+  </si>
+  <si>
+    <t>고대에 설계된 서브카빈으로, 중간장약 소총탄을 사용할 수 있는 화력과 기관단총의 휴대성을 하나로 합쳤습니다.</t>
+  </si>
+  <si>
+    <t>Ancient sub-carbine design, combining the firepower of a potent intermediate cartridge with the compactness of an SMG.</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKMSU.description</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKMSU.description</t>
+  </si>
+  <si>
+    <t>CE_Gun_AKMSU.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_AKMSU.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_SigMCX.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SigMCX.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_SigMCX.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SigMCX.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_SigMCX.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SigMCX.tools.stock.label</t>
+  </si>
+  <si>
+    <t>SIG MCX 돌격 소총</t>
+  </si>
+  <si>
+    <t>SIG MCX</t>
+  </si>
+  <si>
+    <t>CE_Gun_SigMCX.verbs.Verb_ShootCE.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SigMCX.verbs.Verb_ShootCE.label</t>
+  </si>
+  <si>
+    <t>구식 설계의 카빈입니다. 쇼트 스트로크 가스 피스톤 시스템을 사용하여 신뢰성이 높고 반동도 적습니다.</t>
+  </si>
+  <si>
+    <t>An outdated carbine design, featuring a short-stroke gas piston system to improve reliability and reduce recoil.</t>
+  </si>
+  <si>
+    <t>CE_Gun_SigMCX.description</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SigMCX.description</t>
+  </si>
+  <si>
+    <t>CE_Gun_SigMCX.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SigMCX.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_USASTwelve.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_USASTwelve.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_USASTwelve.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_USASTwelve.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_USASTwelve.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_USASTwelve.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_WinchesterNintyFour.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_WinchesterNintyFour.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_WinchesterNintyFour.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_WinchesterNintyFour.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_WinchesterNintyFour.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_WinchesterNintyFour.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_SWGovernor.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SWGovernor.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_SWGovernor.tools.grip.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_SWGovernor.tools.grip.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FlintlockMusket.tools.bayonet.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FlintlockMusket.tools.bayonet.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FlintlockMusket.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FlintlockMusket.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FlintlockMusket.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FlintlockMusket.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FlintlockBlunderbuss.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FlintlockBlunderbuss.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FlintlockBlunderbuss.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FlintlockBlunderbuss.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FlintlockBlunderbuss.tools.stock.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FlintlockBlunderbuss.tools.stock.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FlintlockPistol.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FlintlockPistol.tools.muzzle.label</t>
+  </si>
+  <si>
+    <t>CE_Gun_FlintlockPistol.tools.grip.label</t>
+  </si>
+  <si>
+    <t>ThingDef+CE_Gun_FlintlockPistol.tools.grip.label</t>
+  </si>
+  <si>
+    <t>RecipeDef+Make_Gun_ChainShotgun.label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+Make_Gun_ChainShotgun.description</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+Make_Gun_ChainShotgun.jobString</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saiga 12K 전투 산탄총 제작 중</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>왜 얘만 본편이 아니라 여기 있는거지</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1566,8 +2166,33 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1586,8 +2211,13 @@
         <bgColor rgb="FF87CEEB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1595,19 +2225,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="메모" xfId="3" builtinId="10"/>
+    <cellStyle name="메모 2" xfId="2" xr:uid="{70884ED3-C2E1-468F-98E7-48DB9B1DECFF}"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="1" xr:uid="{D62921CC-0C0E-472A-BBEE-BC1531C280B9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1819,14 +2478,3206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE34443-664C-4E4F-9861-546C21E8B5F3}">
+  <dimension ref="A1:G186"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="65" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>651</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="5" t="s">
+        <v>628</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>627</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="5" t="s">
+        <v>626</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>623</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E143" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F143" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F144" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F145" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="E146" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F146" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F147" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="E148" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F148" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E149" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F149" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="E151" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F151" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F152" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="E153" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F153" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="E154" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F154" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E155" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F155" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E156" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F156" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="E157" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F157" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="E158" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F158" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="E159" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F159" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="E160" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="F160" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="E161" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="F161" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="F162" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="F163" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="F164" s="5" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E165" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="F165" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="F166" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="F167" s="5" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
+      <c r="A168" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="F168" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G168" s="8" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="F169" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G169" s="8"/>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="A170" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="F170" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="G170" s="8"/>
+    </row>
+    <row r="171" spans="1:7">
+      <c r="A171" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="E171" s="5" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
+      <c r="A172" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="E172" s="5" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
+      <c r="A173" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="E173" s="5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
+      <c r="A174" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="D174" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="E174" s="5" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
+      <c r="A175" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="E175" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="G175" s="6" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
+      <c r="A176" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="E176" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="F176" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="G176" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
+      <c r="A177" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C177" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="E177" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="F177" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="G177" s="6"/>
+    </row>
+    <row r="178" spans="1:7">
+      <c r="A178" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="F178" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="G178" s="6"/>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="E179" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="F179" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="G179" s="6"/>
+    </row>
+    <row r="180" spans="1:7">
+      <c r="A180" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="E180" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="F180" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="G180" s="6"/>
+    </row>
+    <row r="181" spans="1:7">
+      <c r="A181" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="E181" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="F181" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="G181" s="6"/>
+    </row>
+    <row r="182" spans="1:7">
+      <c r="A182" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="E182" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="F182" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="G182" s="6"/>
+    </row>
+    <row r="183" spans="1:7">
+      <c r="A183" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="E183" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="F183" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="G183" s="6"/>
+    </row>
+    <row r="184" spans="1:7">
+      <c r="A184" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C184" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="E184" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="F184" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="G184" s="6"/>
+    </row>
+    <row r="185" spans="1:7">
+      <c r="A185" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="E185" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="F185" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="G185" s="6"/>
+    </row>
+    <row r="186" spans="1:7">
+      <c r="A186" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C186" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="E186" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="F186" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="G186" s="6" t="s">
+        <v>505</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1839,7 +5690,7 @@
     <col min="6" max="6" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Combat Extended Guns 수정
#1214
</commit_message>
<xml_diff>
--- a/Data/Combat Extended/①_Combat Extended Guns - 1582570547/1582570547.xlsx
+++ b/Data/Combat Extended/①_Combat Extended Guns - 1582570547/1582570547.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Combat Extended\①_Combat Extended Guns - 1582570547\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB2F9A3-878D-4F5A-A7F3-FF40096C7E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D9A034-D4FF-48EC-BF8A-393F72077E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="38340" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240726" sheetId="2" r:id="rId1"/>
+    <sheet name="Main_240726" sheetId="3" r:id="rId1"/>
     <sheet name="Old_240415" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="697">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -2117,31 +2117,35 @@
     <t>ThingDef+CE_Gun_FlintlockPistol.tools.grip.label</t>
   </si>
   <si>
+    <t>// 직접 추가 필요</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Gun_Minigun.label</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saiga 12K 전투 산탄총 제작 중</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+Make_Gun_ChainShotgun.jobString</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+Make_Gun_ChainShotgun.description</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
     <t>RecipeDef+Make_Gun_ChainShotgun.label</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecipeDef+Make_Gun_ChainShotgun.description</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecipeDef+Make_Gun_ChainShotgun.jobString</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Saiga 12K 전투 산탄총 제작 중</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>왜 얘만 본편이 아니라 여기 있는거지</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2183,13 +2187,6 @@
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2241,17 +2238,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2259,11 +2253,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="메모" xfId="3" builtinId="10"/>
+  <cellStyles count="3">
     <cellStyle name="메모 2" xfId="2" xr:uid="{70884ED3-C2E1-468F-98E7-48DB9B1DECFF}"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="표준 2" xfId="1" xr:uid="{D62921CC-0C0E-472A-BBEE-BC1531C280B9}"/>
@@ -2478,11 +2469,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE34443-664C-4E4F-9861-546C21E8B5F3}">
-  <dimension ref="A1:G186"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B196E705-8C33-47E3-9DFE-22CD3B97BD35}">
+  <dimension ref="A1:G187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17"/>
@@ -5266,6 +5257,9 @@
       <c r="F163" s="5" t="s">
         <v>431</v>
       </c>
+      <c r="G163" s="6" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="164" spans="1:7">
       <c r="A164" s="5" t="s">
@@ -5280,6 +5274,9 @@
       <c r="F164" s="5" t="s">
         <v>522</v>
       </c>
+      <c r="G164" s="6" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="165" spans="1:7">
       <c r="A165" s="5" t="s">
@@ -5311,6 +5308,9 @@
       <c r="F166" s="5" t="s">
         <v>441</v>
       </c>
+      <c r="G166" s="6" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="167" spans="1:7">
       <c r="A167" s="5" t="s">
@@ -5325,10 +5325,13 @@
       <c r="F167" s="5" t="s">
         <v>522</v>
       </c>
+      <c r="G167" s="6" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="168" spans="1:7">
-      <c r="A168" s="7" t="s">
-        <v>691</v>
+      <c r="A168" s="5" t="s">
+        <v>696</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>425</v>
@@ -5339,13 +5342,13 @@
       <c r="F168" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="G168" s="8" t="s">
+      <c r="G168" s="6" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" s="5" t="s">
         <v>695</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7">
-      <c r="A169" s="7" t="s">
-        <v>692</v>
       </c>
       <c r="B169" s="5" t="s">
         <v>425</v>
@@ -5356,11 +5359,13 @@
       <c r="F169" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="G169" s="8"/>
+      <c r="G169" s="6" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="170" spans="1:7">
-      <c r="A170" s="7" t="s">
-        <v>693</v>
+      <c r="A170" s="5" t="s">
+        <v>694</v>
       </c>
       <c r="B170" s="5" t="s">
         <v>425</v>
@@ -5369,9 +5374,11 @@
         <v>451</v>
       </c>
       <c r="F170" s="5" t="s">
-        <v>694</v>
-      </c>
-      <c r="G170" s="8"/>
+        <v>693</v>
+      </c>
+      <c r="G170" s="6" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="171" spans="1:7">
       <c r="A171" s="5" t="s">
@@ -5661,6 +5668,23 @@
       </c>
       <c r="G186" s="6" t="s">
         <v>505</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C187" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="F187" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="G187" s="6" t="s">
+        <v>691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>